<commit_message>
m: fix XLSX -> MD table conversion errors
</commit_message>
<xml_diff>
--- a/docs/n64-mksprite-commands.xlsx
+++ b/docs/n64-mksprite-commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\n64-mksprite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D817523-1BA2-4525-B49A-472500CE5A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE449A3D-C3B7-4AEF-B6AE-A4B938A4810E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8760" yWindow="705" windowWidth="13500" windowHeight="13545" xr2:uid="{1DA2A57C-19A8-45D7-9589-58CD7B970723}"/>
+    <workbookView xWindow="7155" yWindow="2235" windowWidth="13500" windowHeight="13545" xr2:uid="{1DA2A57C-19A8-45D7-9589-58CD7B970723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,15 +146,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>&lt;file|dir&gt;</t>
-  </si>
-  <si>
-    <t>&lt;format&gt;</t>
-  </si>
-  <si>
-    <t>Remove all input files' extensions. Yields files formated as "&lt;file&gt;.sprite"</t>
-  </si>
-  <si>
     <t>Number of slices across the vertical axis (horizontal cuts)</t>
   </si>
   <si>
@@ -164,14 +155,23 @@
     <t>--resampler</t>
   </si>
   <si>
-    <t>&lt;resampler&gt;</t>
-  </si>
-  <si>
     <t>bicubic</t>
   </si>
   <si>
-    <t>The resampler to use when scaling images.
+    <t>[resampler]</t>
+  </si>
+  <si>
+    <t>[format]</t>
+  </si>
+  <si>
+    <t>[file|dir]</t>
+  </si>
+  <si>
+    <t>The resampler to use when scaling images. Argument is case-insensitive.
 Resamplers: Bicubic, Box, CatmullRom, Hermite, Lanczos2, Lanczos3, Lanczos5, Lanczos8, MitchellNetravali, NearestNeighbor, Robidoux, RobidouxSharp, Spline, Triangle, Welch.</t>
+  </si>
+  <si>
+    <t>Remove all input files' extensions. Yields files formated as ".sprite"</t>
   </si>
 </sst>
 </file>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF507966-F155-4812-A906-FEAB6883F125}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
@@ -639,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="2" t="s">
@@ -699,7 +699,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>32</v>
@@ -720,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -767,16 +767,16 @@
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more short commands, update operations table
</commit_message>
<xml_diff>
--- a/docs/n64-mksprite-commands.xlsx
+++ b/docs/n64-mksprite-commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\n64-mksprite\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE449A3D-C3B7-4AEF-B6AE-A4B938A4810E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C61516F-0204-4B58-8B70-EFCC577C0482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7155" yWindow="2235" windowWidth="13500" windowHeight="13545" xr2:uid="{1DA2A57C-19A8-45D7-9589-58CD7B970723}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Short Command</t>
   </si>
@@ -171,7 +171,16 @@
 Resamplers: Bicubic, Box, CatmullRom, Hermite, Lanczos2, Lanczos3, Lanczos5, Lanczos8, MitchellNetravali, NearestNeighbor, Robidoux, RobidouxSharp, Spline, Triangle, Welch.</t>
   </si>
   <si>
-    <t>Remove all input files' extensions. Yields files formated as ".sprite"</t>
+    <t>-h</t>
+  </si>
+  <si>
+    <t>-s</t>
+  </si>
+  <si>
+    <t>-p</t>
+  </si>
+  <si>
+    <t>Remove all input files' extensions. Yields files formated as "*.sprite"</t>
   </si>
 </sst>
 </file>
@@ -227,13 +236,13 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -258,14 +267,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9E2FA813-C7EF-4EB7-82ED-31CAB6310726}" name="Table2" displayName="Table2" ref="A1:E14" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9E2FA813-C7EF-4EB7-82ED-31CAB6310726}" name="Table2" displayName="Table2" ref="A1:E14" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:E14" xr:uid="{9E2FA813-C7EF-4EB7-82ED-31CAB6310726}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0E4BD9D3-B067-4884-BDB1-75DE9D40203B}" name="Short Command" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{19C6681B-8905-4DB6-9B06-EE3F1803090B}" name="Long Comamnd" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{99F02253-0D9B-4479-9666-91AB6FCD29A2}" name="Value" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{79CDF7D5-0119-41E8-AEA1-0153D2707D3F}" name="Default" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{A44CD24A-0CC0-4540-8718-769C50610F8F}" name="Description" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{0E4BD9D3-B067-4884-BDB1-75DE9D40203B}" name="Short Command" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{19C6681B-8905-4DB6-9B06-EE3F1803090B}" name="Long Comamnd" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{99F02253-0D9B-4479-9666-91AB6FCD29A2}" name="Value" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{79CDF7D5-0119-41E8-AEA1-0153D2707D3F}" name="Default" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{A44CD24A-0CC0-4540-8718-769C50610F8F}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -600,9 +609,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -647,7 +654,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -662,7 +671,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
@@ -709,7 +720,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
@@ -724,7 +737,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -791,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>